<commit_message>
Fri Feb 28 06:50:05 AM CST 2025
</commit_message>
<xml_diff>
--- a/bosai/summary_month_2025_2/summary_month.xlsx
+++ b/bosai/summary_month_2025_2/summary_month.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
     <workbookView windowWidth="28800" windowHeight="11355"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$30</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>项目部月报   __生信_ 部 黄礼闯   本月工作完成情况</t>
   </si>
@@ -62,105 +61,6 @@
     <t>备注/遇到问题</t>
   </si>
   <si>
-    <t>BSXL231116</t>
-  </si>
-  <si>
-    <t>千昌石</t>
-  </si>
-  <si>
-    <t>生信协助</t>
-  </si>
-  <si>
-    <t>图片修改</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>BSLL250203</t>
-  </si>
-  <si>
-    <t>王东敏</t>
-  </si>
-  <si>
-    <t>思路设计</t>
-  </si>
-  <si>
-    <t>网络药理学</t>
-  </si>
-  <si>
-    <t>BSJF250113</t>
-  </si>
-  <si>
-    <t>傅兰君</t>
-  </si>
-  <si>
-    <t>生信分析</t>
-  </si>
-  <si>
-    <t>消瘀泄浊饮对糖尿病肾病</t>
-  </si>
-  <si>
-    <t>BSXG250204</t>
-  </si>
-  <si>
-    <t>公司内部</t>
-  </si>
-  <si>
-    <t>多酚五种成分与高脂血症网络药理分析</t>
-  </si>
-  <si>
-    <t>线粒体自噬</t>
-  </si>
-  <si>
-    <t>BSXL240708</t>
-  </si>
-  <si>
-    <t>宛迎春</t>
-  </si>
-  <si>
-    <t>卵巢癌耐药性</t>
-  </si>
-  <si>
-    <t>BS.develop</t>
-  </si>
-  <si>
-    <t>模块开发</t>
-  </si>
-  <si>
-    <t>蛋白质之间互作对接</t>
-  </si>
-  <si>
-    <t>用于 STEINGdb 找不到互作数据的蛋白质对，实现 `ClusPro` 自动准备数据、上传数据</t>
-  </si>
-  <si>
-    <t>Pearson相关分析</t>
-  </si>
-  <si>
-    <t>METTL3、METTL14等表达与预期不符</t>
-  </si>
-  <si>
-    <t>BSGY240816</t>
-  </si>
-  <si>
-    <t>颜艺超</t>
-  </si>
-  <si>
-    <t>结肠癌</t>
-  </si>
-  <si>
-    <t>PIEZO1表达与预期不符</t>
-  </si>
-  <si>
-    <t>BSCL250212</t>
-  </si>
-  <si>
-    <t>董林</t>
-  </si>
-  <si>
-    <t>结肠癌CALM3</t>
-  </si>
-  <si>
     <t>需协调与帮助：暂无</t>
   </si>
   <si>
@@ -176,7 +76,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
@@ -202,24 +102,28 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
       <charset val="0"/>
     </font>
     <font>
       <b/>
       <sz val="16"/>
       <name val="Microsoft YaHei"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Microsoft YaHei"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
       <charset val="0"/>
     </font>
     <font>
@@ -242,6 +146,7 @@
     <font>
       <sz val="14"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
       <charset val="0"/>
     </font>
     <font>
@@ -254,11 +159,13 @@
     <font>
       <sz val="10"/>
       <name val="Microsoft YaHei"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
       <charset val="0"/>
     </font>
     <font>
@@ -269,6 +176,7 @@
     <font>
       <sz val="11"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
       <charset val="0"/>
     </font>
     <font>
@@ -941,7 +849,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -981,12 +889,21 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1008,16 +925,37 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="3" fillId="0" fontId="9" numFmtId="14" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="3" fillId="0" fontId="7" numFmtId="14" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1548,12 +1486,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <sheetPr/>
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:A17"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1561,7 +1499,7 @@
     <col min="1" max="9" width="13.6285714285714" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="22.5" spans="1:9">
+    <row ht="22.5" r="1" spans="1:9">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1572,9 +1510,9 @@
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
-      <c r="I1" s="20"/>
-    </row>
-    <row r="2" ht="33" spans="1:9">
+      <c r="I1" s="23"/>
+    </row>
+    <row ht="33" r="2" spans="1:9">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -1603,520 +1541,758 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" ht="16.5" customHeight="1" spans="1:9">
-      <c r="A3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="17">
+    <row customFormat="1" customHeight="1" ht="16.5" r="3" s="1" spans="1:9">
+      <c r="A3" s="7" t="inlineStr">
+        <is>
+          <t>BSXL231116</t>
+        </is>
+      </c>
+      <c r="B3" s="8" t="inlineStr">
+        <is>
+          <t>千昌石</t>
+        </is>
+      </c>
+      <c r="C3" s="9" t="inlineStr">
+        <is>
+          <t>生信协助</t>
+        </is>
+      </c>
+      <c r="D3" s="8" t="inlineStr">
+        <is>
+          <t>图片修改</t>
+        </is>
+      </c>
+      <c r="E3" s="34">
         <v>45694</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="34">
         <v>45694</v>
       </c>
-      <c r="G3" s="17">
+      <c r="G3" s="34">
         <v>45695</v>
       </c>
-      <c r="H3" s="18">
+      <c r="H3" s="35">
         <v>45695</v>
       </c>
-      <c r="I3" s="21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" s="1" customFormat="1" ht="16.5" customHeight="1" spans="1:9">
-      <c r="A4" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="17">
+      <c r="I3" s="24" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="4" s="1" spans="1:9">
+      <c r="A4" s="7" t="inlineStr">
+        <is>
+          <t>BSLL250203</t>
+        </is>
+      </c>
+      <c r="B4" s="10" t="inlineStr">
+        <is>
+          <t>王东敏</t>
+        </is>
+      </c>
+      <c r="C4" s="9" t="inlineStr">
+        <is>
+          <t>思路设计</t>
+        </is>
+      </c>
+      <c r="D4" s="10" t="inlineStr">
+        <is>
+          <t>网络药理学</t>
+        </is>
+      </c>
+      <c r="E4" s="34">
         <v>45695</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="34">
         <v>45700</v>
       </c>
-      <c r="G4" s="17">
+      <c r="G4" s="34">
         <v>45695</v>
       </c>
-      <c r="H4" s="17">
+      <c r="H4" s="34">
         <v>45695</v>
       </c>
-      <c r="I4" s="21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" s="1" customFormat="1" ht="16.5" customHeight="1" spans="1:9">
-      <c r="A5" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="17">
+      <c r="I4" s="24" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="5" s="1" spans="1:9">
+      <c r="A5" s="7" t="inlineStr">
+        <is>
+          <t>BSJF250113</t>
+        </is>
+      </c>
+      <c r="B5" s="7" t="inlineStr">
+        <is>
+          <t>傅兰君</t>
+        </is>
+      </c>
+      <c r="C5" s="7" t="inlineStr">
+        <is>
+          <t>生信分析</t>
+        </is>
+      </c>
+      <c r="D5" s="10" t="inlineStr">
+        <is>
+          <t>消瘀泄浊饮对糖尿病肾病</t>
+        </is>
+      </c>
+      <c r="E5" s="34">
         <v>45695</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="34">
         <v>45716</v>
       </c>
-      <c r="G5" s="17">
+      <c r="G5" s="34">
         <v>45696</v>
       </c>
-      <c r="H5" s="17">
+      <c r="H5" s="34">
         <v>45696</v>
       </c>
-      <c r="I5" s="21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" s="1" customFormat="1" ht="16.5" customHeight="1" spans="1:9">
-      <c r="A6" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="17">
+      <c r="I5" s="24" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="6" s="1" spans="1:9">
+      <c r="A6" s="7" t="inlineStr">
+        <is>
+          <t>BSXG250204</t>
+        </is>
+      </c>
+      <c r="B6" s="7" t="inlineStr">
+        <is>
+          <t>公司内部</t>
+        </is>
+      </c>
+      <c r="C6" s="7" t="inlineStr">
+        <is>
+          <t>生信分析</t>
+        </is>
+      </c>
+      <c r="D6" s="7" t="inlineStr">
+        <is>
+          <t>多酚五种成分与高脂血症网络药理分析</t>
+        </is>
+      </c>
+      <c r="E6" s="34">
         <v>45698</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="34">
         <v>45698</v>
       </c>
-      <c r="G6" s="17">
+      <c r="G6" s="34">
         <v>45698</v>
       </c>
-      <c r="H6" s="17">
+      <c r="H6" s="34">
         <v>45698</v>
       </c>
-      <c r="I6" s="21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" s="1" customFormat="1" ht="16.5" customHeight="1" spans="1:9">
-      <c r="A7" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="17">
+      <c r="I6" s="24" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="7" s="1" spans="1:9">
+      <c r="A7" s="7" t="inlineStr">
+        <is>
+          <t>BSJF250113</t>
+        </is>
+      </c>
+      <c r="B7" s="7" t="inlineStr">
+        <is>
+          <t>傅兰君</t>
+        </is>
+      </c>
+      <c r="C7" s="11" t="inlineStr">
+        <is>
+          <t>生信协助</t>
+        </is>
+      </c>
+      <c r="D7" s="7" t="inlineStr">
+        <is>
+          <t>线粒体自噬</t>
+        </is>
+      </c>
+      <c r="E7" s="34">
         <v>45695</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="34">
         <v>45702</v>
       </c>
-      <c r="G7" s="17">
+      <c r="G7" s="34">
         <v>45699</v>
       </c>
-      <c r="H7" s="17">
+      <c r="H7" s="34">
         <v>45699</v>
       </c>
-      <c r="I7" s="21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" s="1" customFormat="1" ht="16.5" customHeight="1" spans="1:9">
-      <c r="A8" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="17">
+      <c r="I7" s="24" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="8" s="1" spans="1:9">
+      <c r="A8" s="7" t="inlineStr">
+        <is>
+          <t>BSXL240708</t>
+        </is>
+      </c>
+      <c r="B8" s="7" t="inlineStr">
+        <is>
+          <t>宛迎春</t>
+        </is>
+      </c>
+      <c r="C8" s="7" t="inlineStr">
+        <is>
+          <t>生信分析</t>
+        </is>
+      </c>
+      <c r="D8" s="7" t="inlineStr">
+        <is>
+          <t>卵巢癌耐药性</t>
+        </is>
+      </c>
+      <c r="E8" s="34">
         <v>45698</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="34">
         <v>45698</v>
       </c>
-      <c r="G8" s="17">
+      <c r="G8" s="34">
         <v>45701</v>
       </c>
-      <c r="H8" s="17">
+      <c r="H8" s="34">
         <v>45701</v>
       </c>
-      <c r="I8" s="21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" s="1" customFormat="1" ht="16.5" customHeight="1" spans="1:9">
-      <c r="A9" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="17">
+      <c r="I8" s="24" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="9" s="1" spans="1:9">
+      <c r="A9" s="7" t="inlineStr">
+        <is>
+          <t>BS.develop</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C9" s="7" t="inlineStr">
+        <is>
+          <t>模块开发</t>
+        </is>
+      </c>
+      <c r="D9" s="7" t="inlineStr">
+        <is>
+          <t>蛋白质之间互作对接</t>
+        </is>
+      </c>
+      <c r="E9" s="34">
         <v>45700</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="34">
         <v>45700</v>
       </c>
-      <c r="G9" s="17">
+      <c r="G9" s="34">
         <v>45700</v>
       </c>
-      <c r="H9" s="17">
+      <c r="H9" s="34">
         <v>45700</v>
       </c>
-      <c r="I9" s="21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" s="2" customFormat="1" ht="16.5" customHeight="1" spans="1:9">
-      <c r="A10" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="17">
+      <c r="I9" s="24" t="inlineStr">
+        <is>
+          <t>用于 STEINGdb 找不到互作数据的蛋白质对，实现 `ClusPro` 自动准备数据、上传数据</t>
+        </is>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="10" s="2" spans="1:9">
+      <c r="A10" s="7" t="inlineStr">
+        <is>
+          <t>BSJF250113</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>傅兰君</t>
+        </is>
+      </c>
+      <c r="C10" s="11" t="inlineStr">
+        <is>
+          <t>生信协助</t>
+        </is>
+      </c>
+      <c r="D10" s="7" t="inlineStr">
+        <is>
+          <t>Pearson相关分析</t>
+        </is>
+      </c>
+      <c r="E10" s="34">
         <v>45695</v>
       </c>
-      <c r="F10" s="17">
+      <c r="F10" s="34">
         <v>45705</v>
       </c>
-      <c r="G10" s="17">
+      <c r="G10" s="34">
         <v>45708</v>
       </c>
-      <c r="H10" s="17">
+      <c r="H10" s="34">
         <v>45708</v>
       </c>
-      <c r="I10" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" s="1" customFormat="1" ht="16.5" customHeight="1" spans="1:9">
-      <c r="A11" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="17">
+      <c r="I10" s="25" t="inlineStr">
+        <is>
+          <t>METTL3、METTL14等表达与预期不符</t>
+        </is>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="11" s="1" spans="1:9">
+      <c r="A11" s="7" t="inlineStr">
+        <is>
+          <t>BSGY240816</t>
+        </is>
+      </c>
+      <c r="B11" s="12" t="inlineStr">
+        <is>
+          <t>颜艺超</t>
+        </is>
+      </c>
+      <c r="C11" s="7" t="inlineStr">
+        <is>
+          <t>生信分析</t>
+        </is>
+      </c>
+      <c r="D11" s="7" t="inlineStr">
+        <is>
+          <t>结肠癌</t>
+        </is>
+      </c>
+      <c r="E11" s="34">
         <v>45674</v>
       </c>
-      <c r="F11" s="17">
+      <c r="F11" s="34">
         <v>45678</v>
       </c>
-      <c r="G11" s="17">
+      <c r="G11" s="34">
         <v>45705</v>
       </c>
-      <c r="H11" s="17">
+      <c r="H11" s="34">
         <v>45705</v>
       </c>
-      <c r="I11" s="21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" ht="18" spans="1:9">
-      <c r="A12" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="17">
+      <c r="I11" s="26" t="inlineStr">
+        <is>
+          <t>PIEZO1表达与预期不符</t>
+        </is>
+      </c>
+    </row>
+    <row ht="18" r="12" spans="1:9">
+      <c r="A12" s="7" t="inlineStr">
+        <is>
+          <t>BSCL250212</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>董林</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="inlineStr">
+        <is>
+          <t>思路设计</t>
+        </is>
+      </c>
+      <c r="D12" s="7" t="inlineStr">
+        <is>
+          <t>结肠癌CALM3</t>
+        </is>
+      </c>
+      <c r="E12" s="34">
         <v>45706</v>
       </c>
-      <c r="F12" s="17">
+      <c r="F12" s="34">
         <v>45712</v>
       </c>
-      <c r="G12" s="17">
+      <c r="G12" s="34">
         <v>45708</v>
       </c>
-      <c r="H12" s="17">
+      <c r="H12" s="34">
         <v>45708</v>
       </c>
-      <c r="I12" s="22" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" s="1" customFormat="1" ht="16.5" customHeight="1" spans="1:9">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="21"/>
-    </row>
-    <row r="14" s="1" customFormat="1" ht="16.5" customHeight="1" spans="1:9">
-      <c r="A14" s="7"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="23"/>
-    </row>
-    <row r="15" s="1" customFormat="1" ht="16.5" customHeight="1" spans="1:9">
-      <c r="A15" s="13"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="23"/>
-    </row>
-    <row r="16" s="1" customFormat="1" ht="16.5" customHeight="1" spans="1:9">
+      <c r="I12" s="27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="13" s="1" spans="1:9">
+      <c r="A13" s="7" t="inlineStr">
+        <is>
+          <t>BSXG240327</t>
+        </is>
+      </c>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>陈立茂</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="inlineStr">
+        <is>
+          <t>补充分析</t>
+        </is>
+      </c>
+      <c r="D13" s="7" t="inlineStr">
+        <is>
+          <t>肺癌</t>
+        </is>
+      </c>
+      <c r="E13" s="34">
+        <v>45544</v>
+      </c>
+      <c r="F13" s="34">
+        <v>45611</v>
+      </c>
+      <c r="G13" s="34">
+        <v>45712</v>
+      </c>
+      <c r="H13" s="34">
+        <v>45712</v>
+      </c>
+      <c r="I13" s="26" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="14" s="1" spans="1:9">
+      <c r="A14" s="7" t="inlineStr">
+        <is>
+          <t>BSHQ241042</t>
+        </is>
+      </c>
+      <c r="B14" s="7" t="inlineStr">
+        <is>
+          <t>梁海东</t>
+        </is>
+      </c>
+      <c r="C14" s="7" t="inlineStr">
+        <is>
+          <t>生信分析</t>
+        </is>
+      </c>
+      <c r="D14" s="12" t="inlineStr">
+        <is>
+          <t>骨肉瘤ZDHHC</t>
+        </is>
+      </c>
+      <c r="E14" s="34">
+        <v>45652</v>
+      </c>
+      <c r="F14" s="34">
+        <v>45716</v>
+      </c>
+      <c r="G14" s="34">
+        <v>45713</v>
+      </c>
+      <c r="H14" s="34">
+        <v>45713</v>
+      </c>
+      <c r="I14" s="28" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="15" s="1" spans="1:9">
+      <c r="A15" s="7" t="inlineStr">
+        <is>
+          <t>BSJF241107</t>
+        </is>
+      </c>
+      <c r="B15" s="7" t="inlineStr">
+        <is>
+          <t>许冠华</t>
+        </is>
+      </c>
+      <c r="C15" s="7" t="inlineStr">
+        <is>
+          <t>生信分析</t>
+        </is>
+      </c>
+      <c r="D15" s="12" t="inlineStr">
+        <is>
+          <t>脓毒症发病标志物</t>
+        </is>
+      </c>
+      <c r="E15" s="34">
+        <v>45615</v>
+      </c>
+      <c r="F15" s="34">
+        <v>45709</v>
+      </c>
+      <c r="G15" s="34">
+        <v>45716</v>
+      </c>
+      <c r="H15" s="34">
+        <v>45716</v>
+      </c>
+      <c r="I15" s="28" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row ht="18" r="16" spans="1:9">
       <c r="A16" s="13"/>
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="23"/>
-    </row>
-    <row r="17" customFormat="1" spans="1:9">
-      <c r="A17" s="14"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="29"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="17" s="1" spans="1:9">
+      <c r="A17" s="7"/>
       <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="24"/>
-    </row>
-    <row r="18" customFormat="1" spans="1:9">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="24"/>
-    </row>
-    <row r="19" customFormat="1" spans="1:9">
-      <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="24"/>
-    </row>
-    <row r="20" customFormat="1" spans="1:9">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="24"/>
-    </row>
-    <row r="21" customFormat="1" spans="1:9">
-      <c r="A21" s="14"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="24"/>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-    </row>
-    <row r="24" ht="22.5" spans="1:9">
-      <c r="A24" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="20"/>
-    </row>
-    <row r="25" ht="33" spans="1:9">
-      <c r="A25" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H25" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I25" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" ht="16.5" customHeight="1" spans="1:9">
-      <c r="A26" s="15"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="30"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="18" s="1" spans="1:9">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="30"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="19" s="1" spans="1:9">
+      <c r="A19" s="7"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="30"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="20" s="1" spans="1:9">
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="30"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="21" s="1" spans="1:9">
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="31"/>
+    </row>
+    <row customFormat="1" r="22" spans="1:9">
+      <c r="A22" s="16"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="32"/>
+    </row>
+    <row customFormat="1" r="23" spans="1:9">
+      <c r="A23" s="16"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="32"/>
+    </row>
+    <row customFormat="1" r="24" spans="1:9">
+      <c r="A24" s="16"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="32"/>
+    </row>
+    <row customFormat="1" r="25" spans="1:9">
+      <c r="A25" s="16"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="32"/>
+    </row>
+    <row customFormat="1" r="26" spans="1:9">
+      <c r="A26" s="16"/>
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="25"/>
-    </row>
-    <row r="27" s="3" customFormat="1" spans="1:9">
-      <c r="A27" s="15"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="15"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="32"/>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="16"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
-    </row>
-    <row r="29" ht="28.5" spans="1:9">
-      <c r="A29" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="16"/>
+      <c r="A28" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
+    </row>
+    <row ht="22.5" r="29" spans="1:9">
+      <c r="A29" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="23"/>
+    </row>
+    <row ht="33" r="30" spans="1:9">
+      <c r="A30" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="16.5" r="31" spans="1:9">
+      <c r="A31" s="18"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="33"/>
+    </row>
+    <row customFormat="1" r="32" s="3" spans="1:9">
+      <c r="A32" s="18"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="18"/>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="19"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+    </row>
+    <row ht="28.5" r="34" spans="1:9">
+      <c r="A34" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="19"/>
     </row>
   </sheetData>
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:I25" etc:filterBottomFollowUsedRange="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:I30" etc:filterBottomFollowUsedRange="0">
     <extLst/>
   </autoFilter>
   <mergeCells count="4">
     <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A22:I22"/>
-    <mergeCell ref="A23:I23"/>
-    <mergeCell ref="A24:I24"/>
+    <mergeCell ref="A27:I27"/>
+    <mergeCell ref="A28:I28"/>
+    <mergeCell ref="A29:I29"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Sat Mar  1 06:50:04 AM CST 2025
</commit_message>
<xml_diff>
--- a/bosai/summary_month_2025_2/summary_month.xlsx
+++ b/bosai/summary_month_2025_2/summary_month.xlsx
@@ -1973,12 +1973,12 @@
     <row customFormat="1" customHeight="1" ht="16.5" r="14" s="1" spans="1:9">
       <c r="A14" s="7" t="inlineStr">
         <is>
-          <t>BSHQ241042</t>
+          <t>BSJF241107</t>
         </is>
       </c>
       <c r="B14" s="7" t="inlineStr">
         <is>
-          <t>梁海东</t>
+          <t>许冠华</t>
         </is>
       </c>
       <c r="C14" s="7" t="inlineStr">
@@ -1988,20 +1988,20 @@
       </c>
       <c r="D14" s="12" t="inlineStr">
         <is>
-          <t>骨肉瘤ZDHHC</t>
+          <t>脓毒症发病标志物</t>
         </is>
       </c>
       <c r="E14" s="34">
-        <v>45652</v>
+        <v>45615</v>
       </c>
       <c r="F14" s="34">
+        <v>45709</v>
+      </c>
+      <c r="G14" s="34">
         <v>45716</v>
       </c>
-      <c r="G14" s="34">
-        <v>45713</v>
-      </c>
       <c r="H14" s="34">
-        <v>45713</v>
+        <v>45716</v>
       </c>
       <c r="I14" s="28" t="inlineStr">
         <is>
@@ -2012,12 +2012,12 @@
     <row customFormat="1" customHeight="1" ht="16.5" r="15" s="1" spans="1:9">
       <c r="A15" s="7" t="inlineStr">
         <is>
-          <t>BSJF241107</t>
+          <t>BSHQ241042</t>
         </is>
       </c>
       <c r="B15" s="7" t="inlineStr">
         <is>
-          <t>许冠华</t>
+          <t>梁海东</t>
         </is>
       </c>
       <c r="C15" s="7" t="inlineStr">
@@ -2027,14 +2027,14 @@
       </c>
       <c r="D15" s="12" t="inlineStr">
         <is>
-          <t>脓毒症发病标志物</t>
+          <t>骨肉瘤ZDHHC</t>
         </is>
       </c>
       <c r="E15" s="34">
-        <v>45615</v>
+        <v>45652</v>
       </c>
       <c r="F15" s="34">
-        <v>45709</v>
+        <v>45716</v>
       </c>
       <c r="G15" s="34">
         <v>45716</v>

</xml_diff>